<commit_message>
Deployed 5732395 with MkDocs version: 1.4.2
</commit_message>
<xml_diff>
--- a/syllabus.xlsx
+++ b/syllabus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmt514/Documents/git/CSCI2244Fall23/site/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1E56A6-E7C0-CC43-9EFE-E2414C78D570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769DC7B1-29CF-6F48-8575-6D4E6B8DA6BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16060" yWindow="2080" windowWidth="20960" windowHeight="17440" xr2:uid="{57F24C4A-B835-A44F-B417-EF765F89F2E5}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="17280" windowHeight="21580" xr2:uid="{57F24C4A-B835-A44F-B417-EF765F89F2E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,9 +65,6 @@
     <t>9~11&lt;br/&gt;9/18 - 9/22</t>
   </si>
   <si>
-    <t>9/18 PS3 Due&lt;br/&gt; 9/18 PS4 Release</t>
-  </si>
-  <si>
     <t>Important Distributions&lt;br/&gt;Expected Value</t>
   </si>
   <si>
@@ -80,60 +77,33 @@
     <t>15~17&lt;br/&gt;10/9 - 10/13</t>
   </si>
   <si>
-    <t>10/10 PS6 Release&lt;br/&gt;10/9 Fall Break&lt;br/&gt;10/10 Substitute Monday Schedule</t>
-  </si>
-  <si>
     <t>18~20&lt;br/&gt;10/16 - 10/20</t>
   </si>
   <si>
-    <t>10/16 PS7 Release&lt;br/&gt;10/17 PS6 Due</t>
-  </si>
-  <si>
     <t>21~23&lt;br/&gt;10/23 - 10/27</t>
   </si>
   <si>
-    <t>10/23 PS8 Release&lt;br/&gt;10/23 PS7 Due</t>
-  </si>
-  <si>
     <t>24~26&lt;br/&gt;10/30 - 11/3</t>
   </si>
   <si>
-    <t>10/30 PS9 Release&lt;br/&gt; 10/30 PS8 Due</t>
-  </si>
-  <si>
     <t>27&lt;br/&gt;11/6 - 11/10</t>
   </si>
   <si>
-    <t>11/6 PS9 Due&lt;br/&gt;11/6 Review Section&lt;br/&gt;&lt;b&gt;11/8 Exam 2&lt;/b&gt;</t>
-  </si>
-  <si>
     <t>28~30&lt;br/&gt;11/13 - 11/17</t>
   </si>
   <si>
-    <t>11/13 PS10 Release&lt;br/&gt;</t>
-  </si>
-  <si>
     <t>Markov Chains&lt;br/&gt;Ergodic Markov Chains</t>
   </si>
   <si>
     <t>31&lt;br/&gt;11/20 - 11/24</t>
   </si>
   <si>
-    <t>11/20 PS11 Release&lt;br/&gt;11/20 PS10 Due&lt;br/&gt;11/22-24 Thanksgiving Holidays</t>
-  </si>
-  <si>
     <t>32~34&lt;br/&gt;11/27 - 12/1</t>
   </si>
   <si>
-    <t>12/1 PS12 Release&lt;br/&gt;12/1 PS11 Due</t>
-  </si>
-  <si>
     <t>35~37&lt;br/&gt;12/4 - 12/8</t>
   </si>
   <si>
-    <t>12/8 PS12 Due</t>
-  </si>
-  <si>
     <t>--&lt;br/&gt;12/11 -</t>
   </si>
   <si>
@@ -146,15 +116,6 @@
     <t>&lt;b&gt;(Date TBD) Exam 3&lt;/b&gt;</t>
   </si>
   <si>
-    <t>No class on 9/4 Labor Day&lt;br/&gt;9/4 PS2 Release&lt;br/&gt;&lt;b&gt;9/5&lt;/b&gt; PS1 Due&lt;br/&gt;9/6 Add/Drop Deadline</t>
-  </si>
-  <si>
-    <t>10/2 PS5 Due&lt;br/&gt;10/2 Review Section&lt;br/&gt;10/2 Drop without "W" Deadline&lt;br/&gt;&lt;b&gt;10/4 Exam 1&lt;/b&gt;&lt;br/&gt;10/6 Fall Break</t>
-  </si>
-  <si>
-    <t>9/25 PS4 Due&lt;br/&gt;9/25 PS5 Release&lt;br/&gt;9/27 Sample Exam 1 Release&lt;br/&gt;9/29 Family Weekend</t>
-  </si>
-  <si>
     <t>Week</t>
   </si>
   <si>
@@ -164,9 +125,6 @@
     <t>Random Variables&lt;br/&gt;Conditional Probability</t>
   </si>
   <si>
-    <t>9/11 PS3 Release&lt;br/&gt;&lt;b&gt;9/12&lt;/b&gt; PS2 Due</t>
-  </si>
-  <si>
     <t>Variance&lt;br/&gt;Chernoff Bounds</t>
   </si>
   <si>
@@ -192,6 +150,48 @@
   </si>
   <si>
     <t>Intro to Branching Processes&lt;br/&gt;Intro to Queuing Theory&lt;br/&gt;Intro to Stochastic Process</t>
+  </si>
+  <si>
+    <t>No class on 9/4 Labor Day&lt;br/&gt;&lt;b&gt;9/6&lt;/b&gt; PS1 Due&lt;br/&gt;9/6 PS2 Release&lt;br/&gt;9/6 Add/Drop Deadline</t>
+  </si>
+  <si>
+    <t>9/13 PS2 Due&lt;br/&gt;9/13 PS3 Release</t>
+  </si>
+  <si>
+    <t>9/20 PS3 Due&lt;br/&gt;9/20 PS4 Release</t>
+  </si>
+  <si>
+    <t>9/27 PS4 Due&lt;br/&gt;9/27 Sample Exam 1 Release&lt;br/&gt;9/29 Family Weekend</t>
+  </si>
+  <si>
+    <t>10/2 Review Section&lt;br/&gt;10/2 Drop without "W" Deadline&lt;br/&gt;&lt;b&gt;10/4 Exam 1&lt;/b&gt;&lt;br/&gt;10/6 Fall Break</t>
+  </si>
+  <si>
+    <t>10/9 Fall Break&lt;br/&gt;10/10 PS5 Release&lt;br/&gt;10/10 Substitute Monday Schedule</t>
+  </si>
+  <si>
+    <t>10/18 PS5 Due&lt;br/&gt;10/18 PS6 Release</t>
+  </si>
+  <si>
+    <t>10/25 PS6 Due&lt;br/&gt;10/25 PS7 Release</t>
+  </si>
+  <si>
+    <t>11/1 PS7 Due&lt;br/&gt;11/1 Sample Exam 2 Release</t>
+  </si>
+  <si>
+    <t>11/6 Review Section&lt;br/&gt;&lt;b&gt;11/8 Exam 2&lt;/b&gt;&lt;br/&gt;11/8 PS8 Release</t>
+  </si>
+  <si>
+    <t>11/15 PS8 Due&lt;br/&gt;11/15 PS9 Release</t>
+  </si>
+  <si>
+    <t>11/22-24 Thanksgiving Holidays</t>
+  </si>
+  <si>
+    <t>11/29 PS9 Due&lt;br/&gt;11/29 PS10 Release</t>
+  </si>
+  <si>
+    <t>12/6 PS10 Due&lt;br/&gt;12/6 Sample Final Exam Release</t>
   </si>
 </sst>
 </file>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5088AFD4-06DF-3E49-A393-910CEFC5B4E8}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="198" zoomScaleNormal="198" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="198" zoomScaleNormal="198" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -579,10 +579,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -613,7 +613,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -627,10 +627,10 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -641,10 +641,10 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
         <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -652,13 +652,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -666,10 +666,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -677,13 +677,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -691,13 +691,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -705,13 +705,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -719,13 +719,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -733,13 +733,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -747,13 +747,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -761,13 +761,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -775,13 +775,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -789,29 +789,29 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" t="s">
         <v>30</v>
-      </c>
-      <c r="C16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>